<commit_message>
nuevos jugadores para el pan
</commit_message>
<xml_diff>
--- a/assets/enlaces.xlsx
+++ b/assets/enlaces.xlsx
@@ -4,15 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="24480" windowHeight="14360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$37</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$A$1</definedName>
-  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,124 +19,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>ENLACE</t>
+    <t>CHOCOLATE</t>
   </si>
   <si>
-    <t>FINADO</t>
-  </si>
-  <si>
-    <t>INDEFINIDO</t>
-  </si>
-  <si>
-    <t>BOTELLO</t>
-  </si>
-  <si>
-    <t>NUTRISA</t>
-  </si>
-  <si>
-    <t>CUERNAVACA</t>
-  </si>
-  <si>
-    <t>SULTANA</t>
+    <t>COMBINADO</t>
   </si>
   <si>
     <t>SIN ENLACE</t>
   </si>
   <si>
-    <t>BALTA</t>
-  </si>
-  <si>
-    <t>VICTOR SALAZAR</t>
-  </si>
-  <si>
-    <t>JAVIER/GERARDO</t>
-  </si>
-  <si>
-    <t>GATICA</t>
-  </si>
-  <si>
-    <t>IMELDA</t>
-  </si>
-  <si>
-    <t>GERARDO MONTEMAYOR</t>
-  </si>
-  <si>
-    <t>LIDIA</t>
-  </si>
-  <si>
-    <t>MARTELL</t>
-  </si>
-  <si>
-    <t>DAVID CASTILLO</t>
-  </si>
-  <si>
-    <t>JORGE SANTOS</t>
-  </si>
-  <si>
-    <t>ITZEL</t>
-  </si>
-  <si>
-    <t>RUBEN LEAL</t>
-  </si>
-  <si>
-    <t>VALDEMAR SUR</t>
-  </si>
-  <si>
-    <t>BRIJIDO MORALES</t>
-  </si>
-  <si>
-    <t>BARCENAS</t>
-  </si>
-  <si>
-    <t>CARLOS CHAVEZ</t>
-  </si>
-  <si>
-    <t>CHANO</t>
-  </si>
-  <si>
-    <t>ADRIAN VILLARREAL</t>
-  </si>
-  <si>
-    <t>MARIO</t>
-  </si>
-  <si>
-    <t>ARTURO-TOÑO</t>
-  </si>
-  <si>
-    <t>GUILLERMINA</t>
-  </si>
-  <si>
-    <t>CARLOS ROBLEDO</t>
-  </si>
-  <si>
-    <t>BAJA</t>
-  </si>
-  <si>
-    <t>OSCAR FLORES</t>
-  </si>
-  <si>
-    <t>OBED MEZA</t>
-  </si>
-  <si>
-    <t>ERICKA</t>
-  </si>
-  <si>
-    <t>MARGARITA ARELLANES</t>
-  </si>
-  <si>
-    <t>DIVISIÓN</t>
-  </si>
-  <si>
-    <t>BUSTILLOS</t>
+    <t>VAINILLA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,29 +45,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -178,27 +62,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,200 +399,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="2" t="s">
-        <v>30</v>
+      <c r="A4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="2" t="s">
+      <c r="A5" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eliminar archivos para carga del pan que ya no se ocupan
</commit_message>
<xml_diff>
--- a/assets/enlaces.xlsx
+++ b/assets/enlaces.xlsx
@@ -19,18 +19,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>CHOCOLATE</t>
-  </si>
-  <si>
-    <t>COMBINADO</t>
-  </si>
-  <si>
-    <t>SIN ENLACE</t>
-  </si>
-  <si>
-    <t>VAINILLA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t>ADRIAN VILLARREAL</t>
+  </si>
+  <si>
+    <t>ADRIAN VILLARREAL 2</t>
+  </si>
+  <si>
+    <t>ALBERTO CORONADO</t>
+  </si>
+  <si>
+    <t>ALVARO SUAREZ X</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>CHECO RIVERA</t>
+  </si>
+  <si>
+    <t>CUPULA</t>
+  </si>
+  <si>
+    <t>ELENA</t>
+  </si>
+  <si>
+    <t>ELENA 2</t>
+  </si>
+  <si>
+    <t>EUGENIO BUENO</t>
+  </si>
+  <si>
+    <t>FARAH</t>
+  </si>
+  <si>
+    <t>FARAH 2</t>
+  </si>
+  <si>
+    <t>FAUSTINO</t>
+  </si>
+  <si>
+    <t>FAUSTINO 2</t>
+  </si>
+  <si>
+    <t>FEDERICO</t>
+  </si>
+  <si>
+    <t>FEDERICO 2</t>
+  </si>
+  <si>
+    <t>FINADO</t>
+  </si>
+  <si>
+    <t>INDEFINIDO</t>
+  </si>
+  <si>
+    <t>JAVI</t>
+  </si>
+  <si>
+    <t>JOSE LUIS COINDREAU</t>
+  </si>
+  <si>
+    <t>JOSE MANUEL</t>
+  </si>
+  <si>
+    <t>JOSE MANUEL 2</t>
+  </si>
+  <si>
+    <t>JUAN CONDE</t>
+  </si>
+  <si>
+    <t>JUAN CONDE 2</t>
+  </si>
+  <si>
+    <t>KARINA MORENO</t>
+  </si>
+  <si>
+    <t>MARCELO MARTINEZ</t>
+  </si>
+  <si>
+    <t>MARIANELA</t>
+  </si>
+  <si>
+    <t>MAURO MOLANO</t>
+  </si>
+  <si>
+    <t>MIRIAM ARROYO</t>
+  </si>
+  <si>
+    <t>PEPE DAVALOS</t>
+  </si>
+  <si>
+    <t>RAUL</t>
+  </si>
+  <si>
+    <t>SONDEO</t>
+  </si>
+  <si>
+    <t>SUSY</t>
+  </si>
+  <si>
+    <t>UGO RUIZ</t>
+  </si>
+  <si>
+    <t>VICTOR FUENTES</t>
+  </si>
+  <si>
+    <t>SUSY 2</t>
+  </si>
+  <si>
+    <t>Folio</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
@@ -46,15 +148,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -62,12 +170,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,35 +541,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A5"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>3684</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>3685</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>3686</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3687</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>3688</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>3689</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>3690</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>3691</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>3692</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>3693</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>3694</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>3695</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>3696</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>3697</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>3698</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>3699</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>3700</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>3701</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>3702</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>3703</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>3704</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>3705</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>3706</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>3707</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>3708</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>3709</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>3710</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>3711</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>3712</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>3713</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>3714</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>3715</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>3716</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>3717</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>3718</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>3719</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>